<commit_message>
files amended to adhere to validation rules
</commit_message>
<xml_diff>
--- a/readme_assets/user-stories.xlsx
+++ b/readme_assets/user-stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oli_c\Desktop\MS5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F667B310-9FD5-4DC6-813B-25BF9AE50C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006D2E5C-295E-4A5B-AA05-961AD6AE2DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE1C74E7-7796-46CD-8CAF-E29EC9DFB22C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>I want to be able to…</t>
   </si>
@@ -239,13 +239,25 @@
     <t>come back to the site and make a purchase on these items</t>
   </si>
   <si>
-    <t>Quickly identify celebration type of each product</t>
-  </si>
-  <si>
     <t>shop and see the relevant product types for my shopping needs</t>
   </si>
   <si>
     <t>Site Owner</t>
+  </si>
+  <si>
+    <t>Quickly identify occasion type of each product</t>
+  </si>
+  <si>
+    <t>Oversee all user reviews on the products</t>
+  </si>
+  <si>
+    <t>review and remove any unfair and unneccesary reviews</t>
+  </si>
+  <si>
+    <t>Enter and keep track of the stock levels for each item</t>
+  </si>
+  <si>
+    <t>know when to order more stock in. The site also will show any out of stock products to users</t>
   </si>
 </sst>
 </file>
@@ -611,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19D1A89-BDA5-40B4-B71E-9134C46C330F}">
-  <dimension ref="A2:D35"/>
+  <dimension ref="A2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,7 +631,7 @@
   <cols>
     <col min="1" max="1" width="27.6328125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.453125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="95.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -630,7 +642,7 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -641,6 +653,7 @@
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -649,7 +662,7 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D4" t="s">
@@ -663,7 +676,7 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
@@ -677,7 +690,7 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
@@ -691,11 +704,11 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -705,7 +718,7 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
@@ -719,7 +732,7 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D9" t="s">
@@ -738,7 +751,7 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
@@ -752,7 +765,7 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
@@ -766,7 +779,7 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
@@ -780,7 +793,7 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="s">
@@ -794,7 +807,7 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
@@ -808,7 +821,7 @@
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
@@ -827,7 +840,7 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
@@ -841,7 +854,7 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
@@ -855,7 +868,7 @@
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
@@ -869,7 +882,7 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
@@ -883,7 +896,7 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
@@ -897,7 +910,7 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D23" t="s">
@@ -916,7 +929,7 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D25" t="s">
@@ -930,7 +943,7 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
@@ -944,7 +957,7 @@
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D27" t="s">
@@ -958,7 +971,7 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D28" t="s">
@@ -972,7 +985,7 @@
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D29" t="s">
@@ -986,7 +999,7 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D30" t="s">
@@ -1000,7 +1013,7 @@
       <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D31" t="s">
@@ -1017,9 +1030,9 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D33" t="s">
@@ -1031,9 +1044,9 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D34" t="s">
@@ -1045,13 +1058,41 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>